<commit_message>
added 5 second pause between lines
</commit_message>
<xml_diff>
--- a/input_translate.xlsx
+++ b/input_translate.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t xml:space="preserve">original</t>
   </si>
@@ -148,6 +148,7 @@
         <color rgb="FF000000"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">우리를 죽이지 않는 것은 우리를 더 강하게 만든다</t>
     </r>
@@ -242,6 +243,12 @@
   </si>
   <si>
     <t xml:space="preserve">Life is like a box of chocolates. You never know what you will get.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dahab al-thaalib al-bunni sarie abr al-ghaba lajalab shaheb minn al-maa </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ذهب الثعلب البني السريع عبر الغابة لجلب شاحب من الماء</t>
   </si>
 </sst>
 </file>
@@ -288,6 +295,7 @@
       <color rgb="FF000000"/>
       <name val="Microsoft YaHei"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -390,10 +398,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="54.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="48.18"/>
@@ -637,6 +645,16 @@
       </c>
       <c r="E17" s="0" t="s">
         <v>67</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="1048447" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>